<commit_message>
Ru was changed to PRIVET
</commit_message>
<xml_diff>
--- a/xls/de.xlsx
+++ b/xls/de.xlsx
@@ -28,23 +28,6 @@
     </bk>
   </cellMetadata>
 </metadata>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>hallo</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>en_test</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -91,13 +74,10 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="true"/>
-    </xf>
   </cellXfs>
   <cellStyles>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,30 +409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>